<commit_message>
20230327 IELTS Speaking Preparation
</commit_message>
<xml_diff>
--- a/Listen&Read/雅思听力.xlsx
+++ b/Listen&Read/雅思听力.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/个人数据/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chukexin1/GitHub/work-life-balance/Listen&amp;Read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056D36B7-80AE-AE4F-A633-93FADAB8E552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F016897E-1653-3640-9DB7-E3EEA67C6C90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{FE455072-4836-B640-8311-D30BEC0AA2FB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{FE455072-4836-B640-8311-D30BEC0AA2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="剑8" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="1087">
   <si>
     <t>题号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -20558,12 +20558,1171 @@
     <t xml:space="preserve"> not realized ... Before = surprised</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>area for coffee and an 3____</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exhibition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MAN: Fine. And we'll also need some sort of open area where people can sit and have a cup of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>coffee</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> we'd like to have an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>exhibition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of our products and services there as well, so that'll need to be quite a big space.
+ANGELA: That's fine,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other facilities
+The hotel also has a spa and rooftop 7____</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ANGELA: Sure. And of course, guests can also make use of all the other facilities at the hotel. So we've got a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>spa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> where you can get massages and facials and so on, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> there's </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>a pool up on the roof</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for the use of guests.
+MAN:Great.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>up on the roof = rooftop  楼顶的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Location
+Wilby Street (quite near the sea)		
+near to restaurants and many 10____</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clubs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单复数，注意看题，都提示了many了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ANGELA: Well, it's downtown on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Wilby Street</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, that's quite a small street, and it's </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>not very far from the sea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. And of course if the conference attendees want to go out on the Saturday evening there's </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>a huge choice of places to eat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Then if they want to make a night of it, they can go on to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t xml:space="preserve"> one of the clubs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the area there are a great many to choose from.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the customer services manager 客服经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>complimentary  = free  免费的 (还有赞美的意思)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13-14 Which TWO ways that volunteers can benefit from volunteering are mentioned?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A. learning how to be a part of a team
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>B. having a sense of purpose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. realizing how lucky they are
+D. improved ability at time management
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>E. boosting their employment prospects</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The benefit from volunteering isn't only for the people being helped. Volunteers also gain from it: they're using their skills, to cope with somebody's mental or physical ill health, and volunteering may be </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>a valuable element of their CV when they're applying for jobs:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> employers usually look favourably on someone who's given up time to help others. Significantly, most </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>volunteers feel that what they're doing gives them a purpose in their lives.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> And in my opinion, they're lucky in that respect, as many people don't have that feeling.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E和B都在文中提到了； 后面的in my opinion, they're lucky in that respect 干扰了我选择C项，但是结合上下文，这是修饰答案B的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Volunteers
+15 __F__ Habib            
+16 __A__ Consuela            
+17 __E__ Minh  
+18 __G__ Tanya            
+19 __D__ Alexei            
+20 __C__ Juba      </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意标记关键词；这样才能在听到同义词时第一时间选中答案。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A. overcome </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>physical difficulties</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. rediscover </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>skills</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>not used for a long time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. improve their </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>communication skills</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+D. solve problems </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>independently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>escape isolation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+F. remember </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>past times</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+G. start a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>new hobby</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Habib</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> supports an elderly lady ... ... ... ... . The songs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>take the listeners back to their youth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and for a little while they can forget the difficulties that they face now.
+Our volunteer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Consuela</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is an amazing woman. She </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>has difficulty walking herself,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ... ... ... . By using herself as an example, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Consuela encourages them to walk more and more.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Minh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> visits a young man who </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>lives alone and can't leave his home on his own</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, so he hardly ever saw anyone. But together they go out to the cinema, or to see friends the young man hadn't been able to visit for a long time.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Tanya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> visits an elderly woman once a week. When the woman found out that Tanya is a professional dressmaker, she got interested. Tanya showed her some soft toys she'd made, and the woman decided to try it herself. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>And now she really enjoys it, and spends hours making toys</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. They're not perhaps up to Tanya's standard yet, but she gains a lot of pleasure from doing it.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Alexei</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is ... ... ... , </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>he's helping them to realise that they aren't helpless, and that they can do something themselves</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to improve their situation. 
+And the last volunteer I'll mention, though there are plenty more, is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>Juba</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. She volunteers with a teenage girl with learning difficulties, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>who wasn't very good at talking to other people.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Juba's worked very patiently with her, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>now the girl is far better at expressing herself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and at understanding other people.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It is due to play in a 22____ band competition.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It has been invited to play in the town's 23____</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>They have listened to a talk by a 24____</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joe hopes the band will attend a 26____ next month.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Band members
+27____ flautist       </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regional</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JOE: They aren't really good </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>enough to enter national band competitions, but they're in a regional one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> later in the term. Even if they don't win, and I don't expect them to, hopefully it'll be an incentive for them to try and improve.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发音问题；将enter national 听成了international； 结合后面的but，这里应该填 regional.   原因：他们还不够好去参加全国性的比赛，但是他们呢将要参加地区性的比赛了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carnival</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JOE: Well, now </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>the town council's organising a carnival</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the summer, and the band has been asked to perform. </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两个单词： council  (委员会)    +     carnival  (狂欢节)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JOE: I </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>played a recording</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I came across, of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>a drummer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> talking about how playing in a band had changed his life.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drummer  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词： drummer  鼓手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JOE: That's what l've got in mind. I'm hoping I can take some of the band to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>a parade</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that's going to take place next month.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词：parade  游行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JOE: There's a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>flautist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> who says she loves playing in the band.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t xml:space="preserve"> We rehearse twice a week after school</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t xml:space="preserve"> but she's hardly ever there</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Then she looks for me the next day and gives me a very plausible reason - she says she had to help her mother, or she's been ill, but to be honest, I don't believe her.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词：rehearse 排练  =  rehearsal
+这一题容易填错为E：has a health problem, 但是结束是 I don't believe it. 而且在后面选项E被明确使用了，所以这里应该填D. miss = hardly ever there</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A. makes a lot of mistakes in rehearsals
+B. keeps making unhelpful suggestions
+C. has difficulty with rhythm
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>. misses too many rehearsals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E. has a health problem
+F. doesn't mix with other students</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compositions show a great deal of 32____ and are drawn from various cultural sources</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>energy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Liza Lim's compositions are vibrant and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>full of energy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and she often explores Asian and Australian Aboriginal cultural </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t>sources</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我这里填成了energetic；   a great deal of = full of</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disturbing  引起烦恼的，令人不安的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Tower of Remoteness is performed by piano and 36____</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>The Tower of Remoteness is scored for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线 (正文)"/>
+      </rPr>
+      <t xml:space="preserve"> piano and clarinet.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clarinet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词：clarinet 单簧管</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Olympics
+diversity  多样性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="41">
+  <fonts count="43">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -20852,6 +22011,16 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线 (正文)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线 (正文)"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -20905,7 +22074,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -21022,6 +22191,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -21323,8 +22495,8 @@
       <xdr:rowOff>1266076</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>177799</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>800099</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>215899</xdr:rowOff>
     </xdr:to>
@@ -22278,15 +23450,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="68">
       <c r="A3" s="1" t="s">
@@ -22355,17 +23527,17 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-    </row>
-    <row r="8" spans="1:7" ht="119">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+    </row>
+    <row r="8" spans="1:7" ht="102">
       <c r="A8" s="1" t="s">
         <v>222</v>
       </c>
@@ -22442,15 +23614,15 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:7" ht="136">
       <c r="A14" s="1" t="s">
@@ -22477,18 +23649,18 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-    </row>
-    <row r="17" spans="1:7" ht="85">
-      <c r="A17" s="40" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+    </row>
+    <row r="17" spans="1:7" ht="68">
+      <c r="A17" s="41" t="s">
         <v>157</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -22507,7 +23679,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="68">
-      <c r="A18" s="40"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="1" t="s">
         <v>164</v>
       </c>
@@ -22524,7 +23696,7 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="136">
-      <c r="A19" s="40"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="1" t="s">
         <v>167</v>
       </c>
@@ -22541,7 +23713,7 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="68">
-      <c r="A20" s="40"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="1" t="s">
         <v>172</v>
       </c>
@@ -22558,7 +23730,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="51">
-      <c r="A21" s="40"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="1" t="s">
         <v>158</v>
       </c>
@@ -22575,7 +23747,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="85">
-      <c r="A22" s="40"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="1" t="s">
         <v>159</v>
       </c>
@@ -22683,12 +23855,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="1" t="s">
@@ -22705,7 +23877,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
-      <c r="A3" s="40">
+      <c r="A3" s="41">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -22715,7 +23887,7 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="17">
-      <c r="A4" s="40"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
@@ -22723,7 +23895,7 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="17">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
@@ -22731,7 +23903,7 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="17">
-      <c r="A6" s="40"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="1" t="s">
         <v>42</v>
       </c>
@@ -22739,7 +23911,7 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="17">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
@@ -22747,7 +23919,7 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="17">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
@@ -22755,7 +23927,7 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="34">
-      <c r="A9" s="40"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
@@ -22822,14 +23994,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:6" ht="34">
       <c r="A4" s="2" t="s">
@@ -22869,67 +24041,67 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="65" customHeight="1">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="40"/>
+      <c r="E7" s="41"/>
     </row>
     <row r="8" spans="1:6" ht="17" customHeight="1">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
     </row>
     <row r="9" spans="1:6" ht="54" customHeight="1">
-      <c r="A9" s="40"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="41" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="41" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28" customHeight="1">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="1:6" ht="53" customHeight="1">
-      <c r="A12" s="40"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" spans="1:6" ht="51">
       <c r="A13" s="8" t="s">
@@ -23014,7 +24186,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="58" customHeight="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>97</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -23023,49 +24195,49 @@
       <c r="C19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="41" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="70">
-      <c r="A20" s="40"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" spans="1:5" ht="17">
-      <c r="A21" s="40"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="40"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" spans="1:5" ht="51">
-      <c r="A22" s="40"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="40"/>
+      <c r="D22" s="41"/>
     </row>
     <row r="23" spans="1:5" ht="68">
-      <c r="A23" s="40"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:5" ht="85">
       <c r="A24" s="2" t="s">
@@ -23181,7 +24353,7 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="85">
+    <row r="32" spans="1:5" ht="68">
       <c r="A32" s="2" t="s">
         <v>139</v>
       </c>
@@ -23252,14 +24424,14 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" customHeight="1">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
     </row>
     <row r="41" spans="1:6" ht="85">
       <c r="A41" s="1" t="s">
@@ -23365,14 +24537,14 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" customHeight="1">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
     </row>
     <row r="51" spans="1:6" ht="51">
       <c r="A51" s="1" t="s">
@@ -23402,7 +24574,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="204">
+    <row r="53" spans="1:6" ht="187">
       <c r="A53" s="1" t="s">
         <v>279</v>
       </c>
@@ -23422,7 +24594,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="136">
+    <row r="54" spans="1:6" ht="119">
       <c r="A54" s="1" t="s">
         <v>282</v>
       </c>
@@ -23439,7 +24611,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="372">
+    <row r="55" spans="1:6" ht="356">
       <c r="A55" s="1" t="s">
         <v>287</v>
       </c>
@@ -23481,7 +24653,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="85">
+    <row r="58" spans="1:6" ht="68">
       <c r="A58" s="1" t="s">
         <v>301</v>
       </c>
@@ -23591,14 +24763,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6" ht="51">
       <c r="A2" s="1" t="s">
@@ -23750,14 +24922,14 @@
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="1:6" ht="68">
       <c r="A14" s="1" t="s">
@@ -23872,7 +25044,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="372">
+    <row r="22" spans="1:6" ht="356">
       <c r="A22" s="1" t="s">
         <v>393</v>
       </c>
@@ -23969,14 +25141,14 @@
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
     </row>
     <row r="31" spans="1:6" ht="51">
       <c r="A31" s="1" t="s">
@@ -24048,7 +25220,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="153">
+    <row r="36" spans="1:4" ht="136">
       <c r="A36" s="1" t="s">
         <v>435</v>
       </c>
@@ -24072,7 +25244,7 @@
       <c r="C37" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="43" t="s">
         <v>454</v>
       </c>
     </row>
@@ -24086,7 +25258,7 @@
       <c r="C38" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="D38" s="43"/>
+      <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="51">
       <c r="A39" s="1" t="s">
@@ -24098,7 +25270,7 @@
       <c r="C39" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="D39" s="43"/>
+      <c r="D39" s="44"/>
     </row>
     <row r="40" spans="1:4" ht="102">
       <c r="A40" s="1" t="s">
@@ -24110,7 +25282,7 @@
       <c r="C40" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="D40" s="43"/>
+      <c r="D40" s="44"/>
     </row>
     <row r="41" spans="1:4" ht="85">
       <c r="A41" s="1" t="s">
@@ -24122,7 +25294,7 @@
       <c r="C41" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="D41" s="43"/>
+      <c r="D41" s="44"/>
     </row>
     <row r="42" spans="1:4" ht="113" customHeight="1">
       <c r="A42" s="1" t="s">
@@ -24134,7 +25306,7 @@
       <c r="C42" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="D42" s="43"/>
+      <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="153">
       <c r="A43" s="1" t="s">
@@ -24253,30 +25425,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97061126-B3C2-8648-A26F-0D8FB5091FC0}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="79.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="56.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="24.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6" ht="34">
       <c r="A2" s="1" t="s">
@@ -24418,7 +25591,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="119">
+    <row r="12" spans="1:6" ht="102">
       <c r="A12" s="1" t="s">
         <v>503</v>
       </c>
@@ -24475,14 +25648,14 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="1" t="s">
@@ -24612,31 +25785,211 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-    </row>
-    <row r="37" spans="1:6" ht="16" customHeight="1">
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+    </row>
+    <row r="32" spans="1:6" ht="68">
+      <c r="A32" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="68">
+      <c r="A33" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="68">
+      <c r="A34" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="136">
+      <c r="A35" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="39" customFormat="1" ht="306">
+      <c r="A36" s="39" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="39" customFormat="1" ht="51">
       <c r="A37" s="39" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="39" customFormat="1" ht="34">
+      <c r="A38" s="39" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="39" customFormat="1" ht="34">
+      <c r="A39" s="39" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="39" customFormat="1" ht="34">
+      <c r="A40" s="39" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B40" s="39" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="39" customFormat="1" ht="136">
+      <c r="A41" s="39" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="39" customFormat="1" ht="51">
+      <c r="A42" s="39" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="39" customFormat="1" ht="34">
+      <c r="A43" s="39" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B43" s="39" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16" customHeight="1">
+      <c r="A45" s="40" t="s">
         <v>467</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A45:F45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24662,14 +26015,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:10" ht="34">
       <c r="A2" s="1" t="s">
@@ -24727,7 +26080,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="68">
+    <row r="6" spans="1:10" ht="51">
       <c r="A6" s="1" t="s">
         <v>537</v>
       </c>
@@ -24929,14 +26282,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6" ht="153">
       <c r="A2" s="1" t="s">
@@ -24994,7 +26347,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="136">
+    <row r="6" spans="1:6" ht="119">
       <c r="A6" s="1" t="s">
         <v>582</v>
       </c>
@@ -25008,7 +26361,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="102">
+    <row r="7" spans="1:6" ht="85">
       <c r="A7" s="1" t="s">
         <v>586</v>
       </c>
@@ -25198,14 +26551,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>756</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:6" ht="51">
       <c r="A24" s="1" t="s">
@@ -25321,7 +26674,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="119">
+    <row r="33" spans="1:6" ht="102">
       <c r="A33" s="1" t="s">
         <v>672</v>
       </c>
@@ -25349,7 +26702,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="170">
+    <row r="35" spans="1:6" ht="153">
       <c r="A35" s="1" t="s">
         <v>681</v>
       </c>
@@ -25448,14 +26801,14 @@
       </c>
     </row>
     <row r="43" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="40" t="s">
         <v>755</v>
       </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
     </row>
     <row r="44" spans="1:6" ht="68">
       <c r="A44" s="1" t="s">
@@ -25468,7 +26821,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="204">
+    <row r="45" spans="1:6" ht="187">
       <c r="A45" s="1" t="s">
         <v>711</v>
       </c>
@@ -25518,7 +26871,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="68">
+    <row r="49" spans="1:6" ht="51">
       <c r="A49" s="1" t="s">
         <v>725</v>
       </c>
@@ -25620,14 +26973,14 @@
       </c>
     </row>
     <row r="57" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="40" t="s">
         <v>754</v>
       </c>
-      <c r="B57" s="39"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
     </row>
     <row r="58" spans="1:6" ht="51">
       <c r="A58" s="1" t="s">
@@ -25714,7 +27067,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="34">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="41" t="s">
         <v>782</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -25723,36 +27076,36 @@
       <c r="D64"/>
     </row>
     <row r="65" spans="1:4" ht="17">
-      <c r="A65" s="40"/>
+      <c r="A65" s="41"/>
       <c r="C65" s="1" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="51">
-      <c r="A66" s="40"/>
+      <c r="A66" s="41"/>
       <c r="C66" s="1" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="51">
-      <c r="A67" s="40"/>
+      <c r="A67" s="41"/>
       <c r="C67" s="1" t="s">
         <v>786</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="34">
-      <c r="A68" s="40"/>
+      <c r="A68" s="41"/>
       <c r="C68" s="1" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="51">
-      <c r="A69" s="40"/>
+      <c r="A69" s="41"/>
       <c r="C69" s="1" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="68">
+    <row r="70" spans="1:4" ht="51">
       <c r="A70" s="1" t="s">
         <v>788</v>
       </c>
@@ -25868,14 +27221,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>811</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:10" ht="85">
       <c r="A2" s="26" t="s">
@@ -26170,14 +27523,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="45" t="s">
         <v>875</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
     </row>
     <row r="22" spans="1:6" ht="85">
       <c r="A22" s="1" t="s">
@@ -26460,14 +27813,14 @@
       <c r="D43" s="28"/>
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="42" t="s">
         <v>952</v>
       </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
       <c r="I44" s="31"/>
@@ -26661,24 +28014,24 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>952</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="42" t="s">
         <v>875</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>

</xml_diff>